<commit_message>
Revision gestion des risques
</commit_message>
<xml_diff>
--- a/Documentation/Gestion_Risques.xlsx
+++ b/Documentation/Gestion_Risques.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olaberge\Documents\S5\Projet S5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olaberge\Documents\S5\Projet S5\Repo_Projet_S5\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86AE351-B6E4-4219-9D7A-C4BD06BBA124}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C7EB02-B812-49C8-9223-797B6900620C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4080" xr2:uid="{11A419DB-A2DA-4695-B197-C6917FD91B9B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4080" xr2:uid="{11A419DB-A2DA-4695-B197-C6917FD91B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643D2F9F-3B59-479A-9C84-6738D322D3B7}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>